<commit_message>
Se agrega cuadro para agregar al checklist
- Faltan modificar cosas para que se calcule automaticamente el total
</commit_message>
<xml_diff>
--- a/Etiquetas KG.xlsx
+++ b/Etiquetas KG.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\molino-pos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Documents\molino-pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF68E81B-E019-4383-8CA8-4037CE6CDC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35669061-89C8-47BC-9035-5534F2D1E6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CA55EB31-1C14-4417-9524-54674B8AEAE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CA55EB31-1C14-4417-9524-54674B8AEAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="SP" sheetId="1" r:id="rId1"/>
     <sheet name="KG" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">KG!$A$1:$D$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">KG!$B$1:$E$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SP!$A$1:$B$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
   <si>
     <t>Producto</t>
   </si>
@@ -449,6 +449,15 @@
   </si>
   <si>
     <t>90000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>001s</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,13 +826,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +846,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -852,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>105</v>
       </c>
@@ -867,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>106</v>
       </c>
@@ -882,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -897,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
@@ -912,7 +921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
@@ -927,7 +936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>110</v>
       </c>
@@ -942,7 +951,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
@@ -957,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
@@ -972,7 +981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
@@ -987,7 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>114</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>115</v>
       </c>
@@ -1017,7 +1026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>118</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>119</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
@@ -1107,7 +1116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>122</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>123</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>125</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>126</v>
       </c>
@@ -1182,7 +1191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>127</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>129</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
@@ -1242,7 +1251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>132</v>
       </c>
@@ -1272,7 +1281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>133</v>
       </c>
@@ -1287,7 +1296,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -1302,7 +1311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>135</v>
       </c>
@@ -1326,1475 +1335,1748 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613A9A05-50CB-49C6-A22F-7495D7DE964B}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>100</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">_xlfn.CEILING.MATH(B2/10)</f>
+      <c r="D2">
+        <f t="shared" ref="D2:D33" si="0">_xlfn.CEILING.MATH(C2/10)</f>
         <v>10</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D33" si="1">LEN(A2)</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E33" si="1">LEN(B2)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <f t="shared" si="0"/>
         <v>8.9999999999999998E+27</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>80</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>100</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>45</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>190</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>260</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>50</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>50</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>50</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>140</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>160</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>25</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>23</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>47</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>80</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>450</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>130</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>610</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>32</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>80</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>100</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>100</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>85</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>110</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>145</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>175</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>180</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>600</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>800</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>145</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>160</v>
       </c>
-      <c r="C34">
-        <f t="shared" ref="C34:C65" si="2">_xlfn.CEILING.MATH(B34/10)</f>
+      <c r="D34">
+        <f t="shared" ref="D34:D65" si="2">_xlfn.CEILING.MATH(C34/10)</f>
         <v>16</v>
       </c>
-      <c r="D34">
-        <f t="shared" ref="D34:D65" si="3">LEN(A34)</f>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="3">LEN(B34)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>100</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>100</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>165</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>68</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>80</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>250</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>140</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>345</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>100</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>40</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>140</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>120</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>38</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>35</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>45</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>40</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>50</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>100</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>120</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>55</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>230</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>90</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>50</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>40</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>200</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>120</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>50</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>70</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B63">
+      <c r="C63">
         <v>150</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B64">
+      <c r="C64">
         <v>45</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B65">
+      <c r="C65">
         <v>80</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B66">
+      <c r="C66">
         <v>70</v>
       </c>
-      <c r="C66">
-        <f t="shared" ref="C66:C97" si="4">_xlfn.CEILING.MATH(B66/10)</f>
+      <c r="D66">
+        <f t="shared" ref="D66:D91" si="4">_xlfn.CEILING.MATH(C66/10)</f>
         <v>7</v>
       </c>
-      <c r="D66">
-        <f t="shared" ref="D66:D91" si="5">LEN(A66)</f>
+      <c r="E66">
+        <f t="shared" ref="E66:E91" si="5">LEN(B66)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B67">
+      <c r="C67">
         <v>140</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B68">
+      <c r="C68">
         <v>130</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B69">
+      <c r="C69">
         <v>350</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B70">
+      <c r="C70">
         <v>260</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B71">
+      <c r="C71">
         <v>100</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B72">
+      <c r="C72">
         <v>110</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B73">
+      <c r="C73">
         <v>40</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B74">
+      <c r="C74">
         <v>180</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B75">
+      <c r="C75">
         <v>70</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B76">
+      <c r="C76">
         <v>135</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B77">
+      <c r="C77">
         <v>130</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B78">
+      <c r="C78">
         <v>50</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B79">
+      <c r="C79">
         <v>55</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B80">
+      <c r="C80">
         <v>180</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B81">
+      <c r="C81">
         <v>140</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B82">
+      <c r="C82">
         <v>130</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B83">
+      <c r="C83">
         <v>55</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B84">
+      <c r="C84">
         <v>100</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B85">
+      <c r="C85">
         <v>50</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B86">
+      <c r="C86">
         <v>90</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B87">
+      <c r="C87">
         <v>50</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B88">
+      <c r="C88">
         <v>75</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B89">
+      <c r="C89">
         <v>100</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B90">
+      <c r="C90">
         <v>150</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B91">
+      <c r="C91">
         <v>75</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D91" xr:uid="{613A9A05-50CB-49C6-A22F-7495D7DE964B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D91">
-      <sortCondition ref="A1:A91"/>
+  <autoFilter ref="B1:E91" xr:uid="{613A9A05-50CB-49C6-A22F-7495D7DE964B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E91">
+      <sortCondition ref="B1:B91"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>